<commit_message>
Fix bug in loader and downgrade min python version
</commit_message>
<xml_diff>
--- a/RankedChoiceSample.xlsx
+++ b/RankedChoiceSample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Title1</t>
   </si>
@@ -173,10 +173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -221,62 +221,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E6" s="1" t="n">
         <v>44962</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="F9" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,6 +299,7 @@
         <v>14</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>